<commit_message>
edit of app and add excel version of 1717
</commit_message>
<xml_diff>
--- a/Pedigree data 1717.xlsx
+++ b/Pedigree data 1717.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11012"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kessonmagid/Documents/qmul_r/Pedigree/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kessonovitch/Documents/GitHub/qmul_git/Pedigree/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98EB5F35-DCA7-0B42-BB37-E821A50D91B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B384004B-8024-0740-B617-D331D61B8477}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="540" yWindow="460" windowWidth="25400" windowHeight="14700" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="20">
   <si>
     <t>ID</t>
   </si>
@@ -39,15 +39,9 @@
     <t>sex</t>
   </si>
   <si>
-    <t>rorg</t>
-  </si>
-  <si>
     <t>affected</t>
   </si>
   <si>
-    <t>strain</t>
-  </si>
-  <si>
     <t>GH</t>
   </si>
   <si>
@@ -88,13 +82,16 @@
   </si>
   <si>
     <t>headache</t>
+  </si>
+  <si>
+    <t>diagnosis</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -122,25 +119,30 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="8" tint="-0.249977111117893"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="9" tint="-0.249977111117893"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="6" tint="-0.249977111117893"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -601,18 +603,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -626,25 +626,22 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>8</v>
+      <c r="H1" t="s">
+        <v>11</v>
       </c>
       <c r="I1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2">
         <v>1</v>
       </c>
@@ -658,23 +655,22 @@
         <v>2</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="3">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="3">
-        <v>1</v>
-      </c>
-      <c r="G2" s="3"/>
-      <c r="H2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3">
         <v>2</v>
       </c>
@@ -691,18 +687,17 @@
       <c r="F3" s="3">
         <v>0</v>
       </c>
-      <c r="G3" s="3"/>
-      <c r="H3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4">
         <v>3</v>
       </c>
@@ -719,18 +714,17 @@
       <c r="F4" s="3">
         <v>0</v>
       </c>
-      <c r="G4" s="3"/>
-      <c r="H4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="J4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5">
         <v>4</v>
       </c>
@@ -747,18 +741,17 @@
       <c r="F5" s="3">
         <v>0</v>
       </c>
-      <c r="G5" s="3"/>
-      <c r="H5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6">
         <v>5</v>
       </c>
@@ -775,18 +768,17 @@
       <c r="F6" s="3">
         <v>0</v>
       </c>
-      <c r="G6" s="3"/>
-      <c r="H6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7">
         <v>6</v>
       </c>
@@ -803,18 +795,17 @@
       <c r="F7" s="3">
         <v>0</v>
       </c>
-      <c r="G7" s="3"/>
-      <c r="H7" t="s">
-        <v>12</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8">
         <v>7</v>
       </c>
@@ -831,18 +822,17 @@
       <c r="F8" s="3">
         <v>0</v>
       </c>
-      <c r="G8" s="3"/>
-      <c r="H8" t="s">
-        <v>12</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9">
         <v>8</v>
       </c>
@@ -859,18 +849,17 @@
       <c r="F9" s="3">
         <v>0</v>
       </c>
-      <c r="G9" s="3"/>
-      <c r="H9" t="s">
-        <v>12</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10">
         <v>9</v>
       </c>
@@ -887,18 +876,17 @@
       <c r="F10" s="3">
         <v>0</v>
       </c>
-      <c r="G10" s="3"/>
-      <c r="H10" t="s">
-        <v>12</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11">
         <v>10</v>
       </c>
@@ -915,18 +903,17 @@
       <c r="F11" s="3">
         <v>0</v>
       </c>
-      <c r="G11" s="4"/>
-      <c r="H11" t="s">
-        <v>12</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-      <c r="J11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12">
         <v>11</v>
       </c>
@@ -943,18 +930,17 @@
       <c r="F12" s="3">
         <v>0</v>
       </c>
-      <c r="G12" s="4"/>
-      <c r="H12" t="s">
-        <v>12</v>
-      </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-      <c r="J12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13">
         <v>12</v>
       </c>
@@ -971,18 +957,17 @@
       <c r="F13" s="3">
         <v>0</v>
       </c>
-      <c r="G13" s="4"/>
-      <c r="H13" t="s">
-        <v>12</v>
-      </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-      <c r="J13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14">
         <v>13</v>
       </c>
@@ -999,18 +984,17 @@
       <c r="F14" s="3">
         <v>0</v>
       </c>
-      <c r="G14" s="4"/>
-      <c r="H14" t="s">
-        <v>12</v>
-      </c>
-      <c r="I14">
-        <v>0</v>
-      </c>
-      <c r="J14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G14" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1027,18 +1011,17 @@
       <c r="F15" s="3">
         <v>0</v>
       </c>
-      <c r="G15" s="4"/>
-      <c r="H15" t="s">
-        <v>12</v>
-      </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-      <c r="J15" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1055,18 +1038,17 @@
       <c r="F16" s="3">
         <v>0</v>
       </c>
-      <c r="G16" s="4"/>
+      <c r="G16" t="s">
+        <v>10</v>
+      </c>
       <c r="H16" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="I16" t="s">
-        <v>18</v>
-      </c>
-      <c r="J16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1083,18 +1065,17 @@
       <c r="F17" s="3">
         <v>0</v>
       </c>
-      <c r="G17" s="4"/>
+      <c r="G17" t="s">
+        <v>10</v>
+      </c>
       <c r="H17" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="I17" t="s">
-        <v>18</v>
-      </c>
-      <c r="J17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1111,18 +1092,17 @@
       <c r="F18" s="3">
         <v>0</v>
       </c>
-      <c r="G18" s="4"/>
+      <c r="G18" t="s">
+        <v>10</v>
+      </c>
       <c r="H18" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="I18" t="s">
-        <v>18</v>
-      </c>
-      <c r="J18" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1139,18 +1119,17 @@
       <c r="F19" s="3">
         <v>0</v>
       </c>
-      <c r="G19" s="4"/>
+      <c r="G19" t="s">
+        <v>10</v>
+      </c>
       <c r="H19" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="I19" t="s">
-        <v>18</v>
-      </c>
-      <c r="J19" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1167,18 +1146,17 @@
       <c r="F20" s="3">
         <v>0</v>
       </c>
-      <c r="G20" s="5"/>
-      <c r="H20" t="s">
-        <v>12</v>
-      </c>
-      <c r="I20">
-        <v>0</v>
-      </c>
-      <c r="J20" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G20" t="s">
+        <v>10</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1195,18 +1173,17 @@
       <c r="F21" s="3">
         <v>0</v>
       </c>
-      <c r="G21" s="5"/>
-      <c r="H21" t="s">
-        <v>12</v>
-      </c>
-      <c r="I21">
-        <v>0</v>
-      </c>
-      <c r="J21" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G21" t="s">
+        <v>10</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1220,23 +1197,22 @@
         <v>2</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F22" s="3">
         <v>1</v>
       </c>
-      <c r="G22" s="5"/>
-      <c r="H22" t="s">
-        <v>12</v>
-      </c>
-      <c r="I22">
-        <v>0</v>
-      </c>
-      <c r="J22" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G22" t="s">
+        <v>10</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1253,18 +1229,17 @@
       <c r="F23" s="3">
         <v>0</v>
       </c>
-      <c r="G23" s="5"/>
-      <c r="H23" t="s">
-        <v>12</v>
-      </c>
-      <c r="I23">
-        <v>0</v>
-      </c>
-      <c r="J23" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G23" t="s">
+        <v>10</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1281,18 +1256,17 @@
       <c r="F24" s="3">
         <v>0</v>
       </c>
-      <c r="G24" s="5"/>
-      <c r="H24" t="s">
-        <v>12</v>
-      </c>
-      <c r="I24">
-        <v>0</v>
-      </c>
-      <c r="J24" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G24" t="s">
+        <v>10</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1309,18 +1283,17 @@
       <c r="F25" s="3">
         <v>0</v>
       </c>
-      <c r="G25" s="5"/>
-      <c r="H25" t="s">
-        <v>12</v>
-      </c>
-      <c r="I25">
-        <v>0</v>
-      </c>
-      <c r="J25" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G25" t="s">
+        <v>10</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1337,18 +1310,17 @@
       <c r="F26" s="3">
         <v>0</v>
       </c>
-      <c r="G26" s="5"/>
-      <c r="H26" t="s">
-        <v>12</v>
-      </c>
-      <c r="I26">
-        <v>0</v>
-      </c>
-      <c r="J26" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G26" t="s">
+        <v>10</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1365,18 +1337,17 @@
       <c r="F27" s="3">
         <v>0</v>
       </c>
-      <c r="G27" s="5"/>
-      <c r="H27" t="s">
-        <v>12</v>
-      </c>
-      <c r="I27">
-        <v>0</v>
-      </c>
-      <c r="J27" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G27" t="s">
+        <v>10</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1393,15 +1364,14 @@
       <c r="F28" s="3">
         <v>0</v>
       </c>
-      <c r="G28" s="5"/>
-      <c r="H28" t="s">
-        <v>12</v>
-      </c>
-      <c r="I28">
-        <v>0</v>
-      </c>
-      <c r="J28" t="s">
-        <v>17</v>
+      <c r="G28" t="s">
+        <v>10</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>